<commit_message>
Change Journal Voucher sheet name
</commit_message>
<xml_diff>
--- a/AnnualReports.Web/Content/ExcelTemplates/JournalVoucherReportTemplate.xlsx
+++ b/AnnualReports.Web/Content/ExcelTemplates/JournalVoucherReportTemplate.xlsx
@@ -1,19 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UpWork\Annual Reporting project\SourceCode\annual-reports\AnnualReports.Web\Content\ExcelTemplates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4637DD7-DE23-4571-A7C7-DE0F263E64A3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="328" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="328"/>
   </bookViews>
   <sheets>
-    <sheet name="Warrants" sheetId="1" r:id="rId1"/>
+    <sheet name="Journal Voucher" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -40,7 +34,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -409,14 +403,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Display unmatched funds in Exceptions tab
</commit_message>
<xml_diff>
--- a/AnnualReports.Web/Content/ExcelTemplates/JournalVoucherReportTemplate.xlsx
+++ b/AnnualReports.Web/Content/ExcelTemplates/JournalVoucherReportTemplate.xlsx
@@ -1,20 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UpWork\Annual Reporting project\SourceCode\annual-reports\AnnualReports.Web\Content\ExcelTemplates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CECEFC8-C25E-4C73-8FC2-A207502CF9D0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="328"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="328" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal Voucher" sheetId="1" r:id="rId1"/>
+    <sheet name="Exceptions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Account Number</t>
   </si>
@@ -29,12 +36,27 @@
   </si>
   <si>
     <t>JV Type</t>
+  </si>
+  <si>
+    <t>Fund Id</t>
+  </si>
+  <si>
+    <t>Row Index</t>
+  </si>
+  <si>
+    <t>Sheet Name</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>JV Rule Account</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -403,14 +425,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -446,4 +468,46 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9263D9A4-A8C5-46BB-9DCD-C436DBC6DB19}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Split journal voucher reports into GC & DIST sheets
</commit_message>
<xml_diff>
--- a/AnnualReports.Web/Content/ExcelTemplates/JournalVoucherReportTemplate.xlsx
+++ b/AnnualReports.Web/Content/ExcelTemplates/JournalVoucherReportTemplate.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UpWork\Annual Reporting project\SourceCode\annual-reports\AnnualReports.Web\Content\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CECEFC8-C25E-4C73-8FC2-A207502CF9D0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCB7B56-28FA-4225-8F90-F573B3A51540}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="328" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Journal Voucher" sheetId="1" r:id="rId1"/>
-    <sheet name="Exceptions" sheetId="2" r:id="rId2"/>
+    <sheet name="GC" sheetId="3" r:id="rId1"/>
+    <sheet name="DIST" sheetId="1" r:id="rId2"/>
+    <sheet name="Exceptions" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Account Number</t>
   </si>
@@ -109,12 +110,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -432,7 +432,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277D3BC8-9F80-4788-8AE7-F4708528BA51}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -442,24 +442,24 @@
     <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" customWidth="1"/>
     <col min="5" max="5" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -471,6 +471,45 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9263D9A4-A8C5-46BB-9DCD-C436DBC6DB19}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -487,22 +526,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>